<commit_message>
update raster labelling (mean 3x3 per pixel)
</commit_message>
<xml_diff>
--- a/prediction_result/presentasi/prediksi_presentasi.xlsx
+++ b/prediction_result/presentasi/prediksi_presentasi.xlsx
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -585,7 +585,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -753,7 +753,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -801,7 +801,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -873,7 +873,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -969,7 +969,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -1065,7 +1065,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -1401,7 +1401,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -1605,7 +1605,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -2097,7 +2097,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -2133,7 +2133,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -2157,7 +2157,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -2337,7 +2337,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -2349,7 +2349,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -2373,7 +2373,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -2565,7 +2565,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -2589,7 +2589,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -2625,7 +2625,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -2673,7 +2673,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -2685,7 +2685,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -2721,7 +2721,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -2865,7 +2865,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -3045,7 +3045,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -3165,7 +3165,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -3177,7 +3177,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -3213,7 +3213,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -3249,7 +3249,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -3261,7 +3261,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -3321,7 +3321,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -3369,7 +3369,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -3441,7 +3441,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -3573,7 +3573,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -3621,7 +3621,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -3633,7 +3633,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -3669,7 +3669,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -3705,7 +3705,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -3765,7 +3765,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -3813,7 +3813,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -3837,7 +3837,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -3849,7 +3849,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -3921,7 +3921,7 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -3933,7 +3933,7 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -4005,7 +4005,7 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -4017,7 +4017,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -4029,7 +4029,7 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -4101,7 +4101,7 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -4149,7 +4149,7 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -4185,7 +4185,7 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -4209,7 +4209,7 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -4245,7 +4245,7 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -4257,7 +4257,7 @@
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -4557,7 +4557,7 @@
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -4569,7 +4569,7 @@
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -4593,7 +4593,7 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -4605,7 +4605,7 @@
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -4653,7 +4653,7 @@
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -4689,7 +4689,7 @@
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -4737,7 +4737,7 @@
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -4773,7 +4773,7 @@
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -4797,7 +4797,7 @@
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -4809,7 +4809,7 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -4821,7 +4821,7 @@
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -4833,7 +4833,7 @@
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -4845,7 +4845,7 @@
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -4941,7 +4941,7 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -4965,7 +4965,7 @@
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -5145,7 +5145,7 @@
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -5169,7 +5169,7 @@
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -5241,7 +5241,7 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -5253,7 +5253,7 @@
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -5265,7 +5265,7 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -5277,7 +5277,7 @@
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -5313,7 +5313,7 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -5325,7 +5325,7 @@
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -5337,7 +5337,7 @@
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -5349,7 +5349,7 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -5457,7 +5457,7 @@
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -5517,7 +5517,7 @@
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -5541,7 +5541,7 @@
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -5553,7 +5553,7 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -5601,7 +5601,7 @@
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -5637,7 +5637,7 @@
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -5661,7 +5661,7 @@
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -5745,7 +5745,7 @@
       </c>
       <c r="B443" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -5769,7 +5769,7 @@
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -5817,7 +5817,7 @@
       </c>
       <c r="B449" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -5829,7 +5829,7 @@
       </c>
       <c r="B450" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -5841,7 +5841,7 @@
       </c>
       <c r="B451" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -5865,7 +5865,7 @@
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -5961,7 +5961,7 @@
       </c>
       <c r="B461" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -6009,7 +6009,7 @@
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -6069,7 +6069,7 @@
       </c>
       <c r="B470" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -6165,7 +6165,7 @@
       </c>
       <c r="B478" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -6177,7 +6177,7 @@
       </c>
       <c r="B479" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -6237,7 +6237,7 @@
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -6249,7 +6249,7 @@
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -6345,7 +6345,7 @@
       </c>
       <c r="B493" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -6405,7 +6405,7 @@
       </c>
       <c r="B498" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -6429,7 +6429,7 @@
       </c>
       <c r="B500" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -6453,7 +6453,7 @@
       </c>
       <c r="B502" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -6513,7 +6513,7 @@
       </c>
       <c r="B507" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -6525,7 +6525,7 @@
       </c>
       <c r="B508" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -6537,7 +6537,7 @@
       </c>
       <c r="B509" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -6561,7 +6561,7 @@
       </c>
       <c r="B511" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -6657,7 +6657,7 @@
       </c>
       <c r="B519" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -6789,7 +6789,7 @@
       </c>
       <c r="B530" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -6813,7 +6813,7 @@
       </c>
       <c r="B532" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -6849,7 +6849,7 @@
       </c>
       <c r="B535" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -6885,7 +6885,7 @@
       </c>
       <c r="B538" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -6909,7 +6909,7 @@
       </c>
       <c r="B540" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -7041,7 +7041,7 @@
       </c>
       <c r="B551" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -7053,7 +7053,7 @@
       </c>
       <c r="B552" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -7137,7 +7137,7 @@
       </c>
       <c r="B559" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -7161,7 +7161,7 @@
       </c>
       <c r="B561" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -7173,7 +7173,7 @@
       </c>
       <c r="B562" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -7317,7 +7317,7 @@
       </c>
       <c r="B574" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -7365,7 +7365,7 @@
       </c>
       <c r="B578" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -7449,7 +7449,7 @@
       </c>
       <c r="B585" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -7509,7 +7509,7 @@
       </c>
       <c r="B590" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -7581,7 +7581,7 @@
       </c>
       <c r="B596" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -7629,7 +7629,7 @@
       </c>
       <c r="B600" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -7785,7 +7785,7 @@
       </c>
       <c r="B613" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -7797,7 +7797,7 @@
       </c>
       <c r="B614" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -7905,7 +7905,7 @@
       </c>
       <c r="B623" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -7977,7 +7977,7 @@
       </c>
       <c r="B629" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -8037,7 +8037,7 @@
       </c>
       <c r="B634" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -8049,7 +8049,7 @@
       </c>
       <c r="B635" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -8145,7 +8145,7 @@
       </c>
       <c r="B643" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -8157,7 +8157,7 @@
       </c>
       <c r="B644" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -8241,7 +8241,7 @@
       </c>
       <c r="B651" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -8265,7 +8265,7 @@
       </c>
       <c r="B653" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -8277,7 +8277,7 @@
       </c>
       <c r="B654" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -8361,7 +8361,7 @@
       </c>
       <c r="B661" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -8373,7 +8373,7 @@
       </c>
       <c r="B662" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -8385,7 +8385,7 @@
       </c>
       <c r="B663" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -8409,7 +8409,7 @@
       </c>
       <c r="B665" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -8445,7 +8445,7 @@
       </c>
       <c r="B668" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -8505,7 +8505,7 @@
       </c>
       <c r="B673" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -8517,7 +8517,7 @@
       </c>
       <c r="B674" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -8553,7 +8553,7 @@
       </c>
       <c r="B677" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -8649,7 +8649,7 @@
       </c>
       <c r="B685" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -8661,7 +8661,7 @@
       </c>
       <c r="B686" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -8697,7 +8697,7 @@
       </c>
       <c r="B689" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -8721,7 +8721,7 @@
       </c>
       <c r="B691" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -8805,7 +8805,7 @@
       </c>
       <c r="B698" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -8913,7 +8913,7 @@
       </c>
       <c r="B707" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -8973,7 +8973,7 @@
       </c>
       <c r="B712" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -8997,7 +8997,7 @@
       </c>
       <c r="B714" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -9057,7 +9057,7 @@
       </c>
       <c r="B719" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -9081,7 +9081,7 @@
       </c>
       <c r="B721" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -9105,7 +9105,7 @@
       </c>
       <c r="B723" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -9261,7 +9261,7 @@
       </c>
       <c r="B736" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -9273,7 +9273,7 @@
       </c>
       <c r="B737" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -9285,7 +9285,7 @@
       </c>
       <c r="B738" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -9321,7 +9321,7 @@
       </c>
       <c r="B741" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -9333,7 +9333,7 @@
       </c>
       <c r="B742" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -9357,7 +9357,7 @@
       </c>
       <c r="B744" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -9381,7 +9381,7 @@
       </c>
       <c r="B746" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -9489,7 +9489,7 @@
       </c>
       <c r="B755" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -9513,7 +9513,7 @@
       </c>
       <c r="B757" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -9525,7 +9525,7 @@
       </c>
       <c r="B758" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -9537,7 +9537,7 @@
       </c>
       <c r="B759" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -9549,7 +9549,7 @@
       </c>
       <c r="B760" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -9621,7 +9621,7 @@
       </c>
       <c r="B766" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -9741,7 +9741,7 @@
       </c>
       <c r="B776" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -9765,7 +9765,7 @@
       </c>
       <c r="B778" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -9777,7 +9777,7 @@
       </c>
       <c r="B779" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -9801,7 +9801,7 @@
       </c>
       <c r="B781" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -9861,7 +9861,7 @@
       </c>
       <c r="B786" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -9909,7 +9909,7 @@
       </c>
       <c r="B790" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -9969,7 +9969,7 @@
       </c>
       <c r="B795" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -10017,7 +10017,7 @@
       </c>
       <c r="B799" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -10245,7 +10245,7 @@
       </c>
       <c r="B818" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -10257,7 +10257,7 @@
       </c>
       <c r="B819" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -10269,7 +10269,7 @@
       </c>
       <c r="B820" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -10305,7 +10305,7 @@
       </c>
       <c r="B823" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -10329,7 +10329,7 @@
       </c>
       <c r="B825" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -10377,7 +10377,7 @@
       </c>
       <c r="B829" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -10413,7 +10413,7 @@
       </c>
       <c r="B832" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -10437,7 +10437,7 @@
       </c>
       <c r="B834" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -10461,7 +10461,7 @@
       </c>
       <c r="B836" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -10509,7 +10509,7 @@
       </c>
       <c r="B840" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -10521,7 +10521,7 @@
       </c>
       <c r="B841" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -10581,7 +10581,7 @@
       </c>
       <c r="B846" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -10593,7 +10593,7 @@
       </c>
       <c r="B847" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -10629,7 +10629,7 @@
       </c>
       <c r="B850" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -10641,7 +10641,7 @@
       </c>
       <c r="B851" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -10665,7 +10665,7 @@
       </c>
       <c r="B853" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -10701,7 +10701,7 @@
       </c>
       <c r="B856" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -10737,7 +10737,7 @@
       </c>
       <c r="B859" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -10773,7 +10773,7 @@
       </c>
       <c r="B862" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -10869,7 +10869,7 @@
       </c>
       <c r="B870" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -10905,7 +10905,7 @@
       </c>
       <c r="B873" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -10917,7 +10917,7 @@
       </c>
       <c r="B874" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -10929,7 +10929,7 @@
       </c>
       <c r="B875" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -10953,7 +10953,7 @@
       </c>
       <c r="B877" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -10965,7 +10965,7 @@
       </c>
       <c r="B878" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -11037,7 +11037,7 @@
       </c>
       <c r="B884" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -11085,7 +11085,7 @@
       </c>
       <c r="B888" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -11097,7 +11097,7 @@
       </c>
       <c r="B889" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -11109,7 +11109,7 @@
       </c>
       <c r="B890" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -11229,7 +11229,7 @@
       </c>
       <c r="B900" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -11241,7 +11241,7 @@
       </c>
       <c r="B901" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -11265,7 +11265,7 @@
       </c>
       <c r="B903" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -11325,7 +11325,7 @@
       </c>
       <c r="B908" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -11349,7 +11349,7 @@
       </c>
       <c r="B910" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -11373,7 +11373,7 @@
       </c>
       <c r="B912" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -11421,7 +11421,7 @@
       </c>
       <c r="B916" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -11445,7 +11445,7 @@
       </c>
       <c r="B918" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -11481,7 +11481,7 @@
       </c>
       <c r="B921" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -11565,7 +11565,7 @@
       </c>
       <c r="B928" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -11577,7 +11577,7 @@
       </c>
       <c r="B929" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -11613,7 +11613,7 @@
       </c>
       <c r="B932" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -11661,7 +11661,7 @@
       </c>
       <c r="B936" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -11673,7 +11673,7 @@
       </c>
       <c r="B937" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -11733,7 +11733,7 @@
       </c>
       <c r="B942" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -11781,7 +11781,7 @@
       </c>
       <c r="B946" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -11925,7 +11925,7 @@
       </c>
       <c r="B958" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -11937,7 +11937,7 @@
       </c>
       <c r="B959" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -11985,7 +11985,7 @@
       </c>
       <c r="B963" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -12033,7 +12033,7 @@
       </c>
       <c r="B967" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -12141,7 +12141,7 @@
       </c>
       <c r="B976" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -12249,7 +12249,7 @@
       </c>
       <c r="B985" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -12285,7 +12285,7 @@
       </c>
       <c r="B988" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -12297,7 +12297,7 @@
       </c>
       <c r="B989" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -12369,7 +12369,7 @@
       </c>
       <c r="B995" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -12393,7 +12393,7 @@
       </c>
       <c r="B997" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -12429,7 +12429,7 @@
       </c>
       <c r="B1000" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -12441,7 +12441,7 @@
       </c>
       <c r="B1001" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -12453,7 +12453,7 @@
       </c>
       <c r="B1002" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -12465,7 +12465,7 @@
       </c>
       <c r="B1003" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -12489,7 +12489,7 @@
       </c>
       <c r="B1005" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -12513,7 +12513,7 @@
       </c>
       <c r="B1007" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -12561,7 +12561,7 @@
       </c>
       <c r="B1011" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -12597,7 +12597,7 @@
       </c>
       <c r="B1014" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -12633,7 +12633,7 @@
       </c>
       <c r="B1017" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -12657,7 +12657,7 @@
       </c>
       <c r="B1019" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -12681,7 +12681,7 @@
       </c>
       <c r="B1021" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -12693,7 +12693,7 @@
       </c>
       <c r="B1022" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -12729,7 +12729,7 @@
       </c>
       <c r="B1025" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -12741,7 +12741,7 @@
       </c>
       <c r="B1026" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -12849,7 +12849,7 @@
       </c>
       <c r="B1035" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -12885,7 +12885,7 @@
       </c>
       <c r="B1038" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -12981,7 +12981,7 @@
       </c>
       <c r="B1046" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -12993,7 +12993,7 @@
       </c>
       <c r="B1047" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -13053,7 +13053,7 @@
       </c>
       <c r="B1052" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -13065,7 +13065,7 @@
       </c>
       <c r="B1053" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -13161,7 +13161,7 @@
       </c>
       <c r="B1061" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -13209,7 +13209,7 @@
       </c>
       <c r="B1065" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -13233,7 +13233,7 @@
       </c>
       <c r="B1067" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -13245,7 +13245,7 @@
       </c>
       <c r="B1068" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -13305,7 +13305,7 @@
       </c>
       <c r="B1073" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -13317,7 +13317,7 @@
       </c>
       <c r="B1074" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -13461,7 +13461,7 @@
       </c>
       <c r="B1086" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -13545,7 +13545,7 @@
       </c>
       <c r="B1093" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -13569,7 +13569,7 @@
       </c>
       <c r="B1095" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -13581,7 +13581,7 @@
       </c>
       <c r="B1096" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -13593,7 +13593,7 @@
       </c>
       <c r="B1097" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -13629,7 +13629,7 @@
       </c>
       <c r="B1100" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -13701,7 +13701,7 @@
       </c>
       <c r="B1106" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -13713,7 +13713,7 @@
       </c>
       <c r="B1107" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -13845,7 +13845,7 @@
       </c>
       <c r="B1118" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -13869,7 +13869,7 @@
       </c>
       <c r="B1120" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -13941,7 +13941,7 @@
       </c>
       <c r="B1126" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -13965,7 +13965,7 @@
       </c>
       <c r="B1128" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -13977,7 +13977,7 @@
       </c>
       <c r="B1129" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -14085,7 +14085,7 @@
       </c>
       <c r="B1138" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -14097,7 +14097,7 @@
       </c>
       <c r="B1139" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -14181,7 +14181,7 @@
       </c>
       <c r="B1146" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -14253,7 +14253,7 @@
       </c>
       <c r="B1152" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -14289,7 +14289,7 @@
       </c>
       <c r="B1155" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -14301,7 +14301,7 @@
       </c>
       <c r="B1156" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -14313,7 +14313,7 @@
       </c>
       <c r="B1157" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -14445,7 +14445,7 @@
       </c>
       <c r="B1168" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -14493,7 +14493,7 @@
       </c>
       <c r="B1172" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -14553,7 +14553,7 @@
       </c>
       <c r="B1177" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -14565,7 +14565,7 @@
       </c>
       <c r="B1178" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -14613,7 +14613,7 @@
       </c>
       <c r="B1182" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -14625,7 +14625,7 @@
       </c>
       <c r="B1183" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -14649,7 +14649,7 @@
       </c>
       <c r="B1185" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -14697,7 +14697,7 @@
       </c>
       <c r="B1189" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -14709,7 +14709,7 @@
       </c>
       <c r="B1190" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -14721,7 +14721,7 @@
       </c>
       <c r="B1191" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -14733,7 +14733,7 @@
       </c>
       <c r="B1192" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -14769,7 +14769,7 @@
       </c>
       <c r="B1195" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -14865,7 +14865,7 @@
       </c>
       <c r="B1203" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -15009,7 +15009,7 @@
       </c>
       <c r="B1215" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -15021,7 +15021,7 @@
       </c>
       <c r="B1216" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -15045,7 +15045,7 @@
       </c>
       <c r="B1218" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -15141,7 +15141,7 @@
       </c>
       <c r="B1226" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -15153,7 +15153,7 @@
       </c>
       <c r="B1227" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -15165,7 +15165,7 @@
       </c>
       <c r="B1228" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -15225,7 +15225,7 @@
       </c>
       <c r="B1233" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -15273,7 +15273,7 @@
       </c>
       <c r="B1237" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -15297,7 +15297,7 @@
       </c>
       <c r="B1239" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -15345,7 +15345,7 @@
       </c>
       <c r="B1243" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -15357,7 +15357,7 @@
       </c>
       <c r="B1244" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -15381,7 +15381,7 @@
       </c>
       <c r="B1246" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -15417,7 +15417,7 @@
       </c>
       <c r="B1249" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -15537,7 +15537,7 @@
       </c>
       <c r="B1259" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -15657,7 +15657,7 @@
       </c>
       <c r="B1269" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -15717,7 +15717,7 @@
       </c>
       <c r="B1274" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -15753,7 +15753,7 @@
       </c>
       <c r="B1277" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -15777,7 +15777,7 @@
       </c>
       <c r="B1279" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -15801,7 +15801,7 @@
       </c>
       <c r="B1281" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -15813,7 +15813,7 @@
       </c>
       <c r="B1282" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -15861,7 +15861,7 @@
       </c>
       <c r="B1286" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -15885,7 +15885,7 @@
       </c>
       <c r="B1288" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -15909,7 +15909,7 @@
       </c>
       <c r="B1290" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -15933,7 +15933,7 @@
       </c>
       <c r="B1292" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -15957,7 +15957,7 @@
       </c>
       <c r="B1294" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -15981,7 +15981,7 @@
       </c>
       <c r="B1296" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -15993,7 +15993,7 @@
       </c>
       <c r="B1297" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -16077,7 +16077,7 @@
       </c>
       <c r="B1304" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -16089,7 +16089,7 @@
       </c>
       <c r="B1305" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -16113,7 +16113,7 @@
       </c>
       <c r="B1307" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -16137,7 +16137,7 @@
       </c>
       <c r="B1309" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -16173,7 +16173,7 @@
       </c>
       <c r="B1312" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -16197,7 +16197,7 @@
       </c>
       <c r="B1314" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -16221,7 +16221,7 @@
       </c>
       <c r="B1316" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -16245,7 +16245,7 @@
       </c>
       <c r="B1318" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -16305,7 +16305,7 @@
       </c>
       <c r="B1323" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -16317,7 +16317,7 @@
       </c>
       <c r="B1324" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -16329,7 +16329,7 @@
       </c>
       <c r="B1325" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -16353,7 +16353,7 @@
       </c>
       <c r="B1327" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -16377,7 +16377,7 @@
       </c>
       <c r="B1329" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -16401,7 +16401,7 @@
       </c>
       <c r="B1331" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -16425,7 +16425,7 @@
       </c>
       <c r="B1333" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -16509,7 +16509,7 @@
       </c>
       <c r="B1340" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -16557,7 +16557,7 @@
       </c>
       <c r="B1344" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -16593,7 +16593,7 @@
       </c>
       <c r="B1347" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -16665,7 +16665,7 @@
       </c>
       <c r="B1353" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -16713,7 +16713,7 @@
       </c>
       <c r="B1357" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -16725,7 +16725,7 @@
       </c>
       <c r="B1358" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -16749,7 +16749,7 @@
       </c>
       <c r="B1360" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -16761,7 +16761,7 @@
       </c>
       <c r="B1361" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -16821,7 +16821,7 @@
       </c>
       <c r="B1366" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -16833,7 +16833,7 @@
       </c>
       <c r="B1367" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>
@@ -16929,7 +16929,7 @@
       </c>
       <c r="B1375" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -16989,7 +16989,7 @@
       </c>
       <c r="B1380" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -17073,7 +17073,7 @@
       </c>
       <c r="B1387" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -17085,7 +17085,7 @@
       </c>
       <c r="B1388" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -17097,7 +17097,7 @@
       </c>
       <c r="B1389" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -17169,7 +17169,7 @@
       </c>
       <c r="B1395" t="inlineStr">
         <is>
-          <t>bangunan</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -17265,7 +17265,7 @@
       </c>
       <c r="B1403" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>air</t>
         </is>
       </c>
     </row>
@@ -17277,7 +17277,7 @@
       </c>
       <c r="B1404" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>area_hijau</t>
         </is>
       </c>
     </row>
@@ -17301,7 +17301,7 @@
       </c>
       <c r="B1406" t="inlineStr">
         <is>
-          <t>area_hijau</t>
+          <t>bangunan</t>
         </is>
       </c>
     </row>

</xml_diff>